<commit_message>
Code refine and add mult-visitor cases
1. Refine Test_simular.py to handle different running cases more clearly.
2. Add multi-visitor behaviours and move it to Visitor_behaivour class.
</commit_message>
<xml_diff>
--- a/train_log/convert_chart.xlsx
+++ b/train_log/convert_chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD9F9D6-116B-4DF6-A4DE-B32B59809211}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941391EF-2132-4A4C-A494-20AC2E8965CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -459,11 +459,11 @@
       </c>
       <c r="C3">
         <f>C2*C4</f>
-        <v>8.8000000000000007</v>
+        <v>25.9</v>
       </c>
       <c r="D3">
         <f>C3/B3</f>
-        <v>0.88000000000000012</v>
+        <v>2.59</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -480,11 +480,11 @@
         <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.88</v>
+        <v>2.59</v>
       </c>
       <c r="D4">
         <f>C4/B4</f>
-        <v>1.76</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -513,11 +513,11 @@
       </c>
       <c r="C8">
         <f>B3/C3</f>
-        <v>1.1363636363636362</v>
+        <v>0.38610038610038611</v>
       </c>
       <c r="D8">
         <f>C8/B8</f>
-        <v>1.1363636363636362</v>
+        <v>0.38610038610038611</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>